<commit_message>
Changes in styles provided by rogal.
</commit_message>
<xml_diff>
--- a/doc/osmapa-garmin.xlsx
+++ b/doc/osmapa-garmin.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873CA023-DA77-4AE6-A08F-96340A3476FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FCDEE7-FD8B-4BC2-812B-CE406BB36637}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="168">
   <si>
     <t>Pobierz</t>
   </si>
@@ -520,6 +520,12 @@
   </si>
   <si>
     <t>{dane_osm}\\srtm_polska.pbf</t>
+  </si>
+  <si>
+    <t>21{fid}001</t>
+  </si>
+  <si>
+    <t>21{fid}000</t>
   </si>
 </sst>
 </file>
@@ -930,9 +936,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X31" sqref="X31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,10 +1817,10 @@
         <v>70</v>
       </c>
       <c r="X28" t="s">
-        <v>63</v>
+        <v>166</v>
       </c>
       <c r="Y28" t="s">
-        <v>65</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1827,8 +1833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADDE2A7-CDFA-4D13-ACD7-212D5F91D52B}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,7 +2266,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added comments and documentation.
</commit_message>
<xml_diff>
--- a/doc/osmapa-garmin.xlsx
+++ b/doc/osmapa-garmin.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FCDEE7-FD8B-4BC2-812B-CE406BB36637}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC63340F-2E16-49F7-AC18-477CF791E1D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
-    <sheet name="compile" sheetId="2" r:id="rId2"/>
-    <sheet name="split" sheetId="3" r:id="rId3"/>
+    <sheet name="Identyfikatory" sheetId="4" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="1" r:id="rId2"/>
+    <sheet name="compile" sheetId="2" r:id="rId3"/>
+    <sheet name="split" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="225">
   <si>
     <t>Pobierz</t>
   </si>
@@ -526,13 +527,191 @@
   </si>
   <si>
     <t>21{fid}000</t>
+  </si>
+  <si>
+    <t>family-id</t>
+  </si>
+  <si>
+    <t>family-name</t>
+  </si>
+  <si>
+    <t>product-id</t>
+  </si>
+  <si>
+    <t>product-version</t>
+  </si>
+  <si>
+    <t>If you build several maps, this option describes the family name of all of your maps. Garmin will display this in the map selection screen. The default is "OSM map".</t>
+  </si>
+  <si>
+    <t>The version of the product. Default value is 100 which means version 1.00.</t>
+  </si>
+  <si>
+    <t>area-name</t>
+  </si>
+  <si>
+    <t>Area name is displayed on Garmin units (or at least on eTrex) as the second part of the mapname in the list of the individual maps.</t>
+  </si>
+  <si>
+    <t>overview-mapname</t>
+  </si>
+  <si>
+    <t>{map_name}</t>
+  </si>
+  <si>
+    <t>{fid}</t>
+  </si>
+  <si>
+    <t>{publisher_id}{fid}001</t>
+  </si>
+  <si>
+    <t>{publisher_id}{fid}000</t>
+  </si>
+  <si>
+    <t>{style}</t>
+  </si>
+  <si>
+    <t>Parameters used</t>
+  </si>
+  <si>
+    <t>OSMapaPL-PODSTAWOWA</t>
+  </si>
+  <si>
+    <t>OSMapaPL-WARSTWICE</t>
+  </si>
+  <si>
+    <t>OSMapaPLext-PODSTAWOWA</t>
+  </si>
+  <si>
+    <t>OSMapaPLext-OGONKI</t>
+  </si>
+  <si>
+    <t>OSMapaPLext-LIGHT</t>
+  </si>
+  <si>
+    <t>OSMapaPLext-WARSTWICE</t>
+  </si>
+  <si>
+    <t>OSMapaPLext-SZLAKI</t>
+  </si>
+  <si>
+    <t>OSMapaPLtest-PODSTAWOWA</t>
+  </si>
+  <si>
+    <t>OSMapaPLtest-OGONKI</t>
+  </si>
+  <si>
+    <t>OSMapaPLtest-LIGHT</t>
+  </si>
+  <si>
+    <t>OSMapaPLtest-WARSTWICE</t>
+  </si>
+  <si>
+    <t>OSMapaPLtest-SZLAKI</t>
+  </si>
+  <si>
+    <t>country-name</t>
+  </si>
+  <si>
+    <t>Set the map's country name. The default is "COUNTRY".</t>
+  </si>
+  <si>
+    <t>country-abbr</t>
+  </si>
+  <si>
+    <t>Set the map's abbreviated country name. The default is "ABC".</t>
+  </si>
+  <si>
+    <t>overview-mapnumber</t>
+  </si>
+  <si>
+    <t>If --tdbfile is enabled, this gives the internal 8 digit number used in the overview map and tdb file. The default number is 63240000.</t>
+  </si>
+  <si>
+    <t>If --tdbfile is enabled, this gives the name of the overview .img and .tdb files. The default map name is osmmap.</t>
+  </si>
+  <si>
+    <t>Specify a style name. Must be used if --style-file points to a location containing multiple styles. If used without also specifying --style-file, it selects one of the built-in styles.</t>
+  </si>
+  <si>
+    <t>Set the name of the map. Garmin maps are identified by an 8 digit number. The default is 63240001. It is best to use a different name if you are going to be making a map for others to use so that it is unique and does not clash with others.
+Change the name of the map (i.e. the name of the output file). Garmin maps are named by 8 digit numbers - each tile that is loaded into a GPS must have a different mapname. The default is 63240001.img. Enter the number only, not the extension (img), otherwise mkgmap will throw an exception.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set the descriptive text for individual tiles and gmapsupp.img. Map tiles take the most recent --description before the --input-file option that defines the tile. Because gmapsupp.img is created after all the other tiles have been processed, gmapsupp.img takes the last --description found in the command line, regardless of where the --gmapsupp option is placed in the command line.
+Note that if you use splitter with its --geonames-file option or its own --description option, the generated template.args file includes --description values that will apply to individual tiles. In this case it is not possible to override splitter's description for individual tiles from the mkgmap command line. Placing the mkgmap --description option after -c template.args ensures that the value is applied to gmapsupp.img.
+Different GPS devices and PC programs handle descriptions inconsistently. Some display the description when selecting maps or tiles, others use the family name.
+Sets the descriptive text for the map. This may be displayed in QLandkarte, MapSource or on a GPS etc. Within the GPS unit, under Maps-&gt;Set-up map you will see that each map tile is labelled with whatever you set in --description. Maximum 20 characters. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is an integer that identifies a family of products. Range: [1..65535] Default: 6324.
+This is an integer that identifies a family of products. If you want to compile a map with a TYP file, you will need to ensure that the family-id of the map matches that of the TYP file. Only one mapset at a time can have the same family-id in Mapsource. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is an integer that identifies a product within a family. It is often just 1, which is the default.
+Each mapset needs an unique product-id in order to let MapSource differentiate between the different maps. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This name will be displayed by Garmin PC programs in the map selection drop-down. The default is "OSM map".
+This is the name displayed in the 'Select a Product' drop down list in MapSource. If you plan to distribute maps using installers then providing a short map description here is very useful. Default is "OSM map". This value is not transferred to the GPS. When loading multiple maps into QLandkarteGT, each map must have a unique series name, otherwise each map will appear identical to the first map loaded. </t>
+  </si>
+  <si>
+    <t>{typfile}</t>
+  </si>
+  <si>
+    <t>[typfile]</t>
+  </si>
+  <si>
+    <t>{mapa_root}/config/{configfile}</t>
+  </si>
+  <si>
+    <t>osmapa.config</t>
+  </si>
+  <si>
+    <t>osmapa_ogonki.config</t>
+  </si>
+  <si>
+    <t>osmapa_light.config</t>
+  </si>
+  <si>
+    <t>osmapa_szlaki.config</t>
+  </si>
+  <si>
+    <t>osmapa_warstwice.config</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>POLAND</t>
+  </si>
+  <si>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>5301</t>
+  </si>
+  <si>
+    <t>5302</t>
+  </si>
+  <si>
+    <t>5303</t>
+  </si>
+  <si>
+    <t>5351</t>
+  </si>
+  <si>
+    <t>5352</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,8 +787,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -622,8 +847,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -631,11 +862,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -654,6 +965,72 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -933,10 +1310,1135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C910433-F3A5-4348-B29A-FC30EC5AEA2B}">
+  <dimension ref="A1:P28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="59.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="18" customFormat="1" ht="375" x14ac:dyDescent="0.25">
+      <c r="B1" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" t="s">
+        <v>177</v>
+      </c>
+      <c r="H3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" t="s">
+        <v>179</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="K3" s="33"/>
+      <c r="L3" t="s">
+        <v>210</v>
+      </c>
+      <c r="M3" t="s">
+        <v>181</v>
+      </c>
+      <c r="N3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" s="37"/>
+      <c r="F4" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="I4" s="40" t="str">
+        <f>_xlfn.CONCAT("66",B4,"001")</f>
+        <v>66004001</v>
+      </c>
+      <c r="J4" s="43" t="str">
+        <f>_xlfn.CONCAT("66",B4,"000")</f>
+        <v>66004000</v>
+      </c>
+      <c r="K4" s="34"/>
+      <c r="L4" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="O4" s="26"/>
+      <c r="P4" s="27"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="E5" s="38"/>
+      <c r="F5" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" s="41" t="str">
+        <f t="shared" ref="I5:I13" si="0">_xlfn.CONCAT("66",B5,"001")</f>
+        <v>66005001</v>
+      </c>
+      <c r="J5" s="44" t="str">
+        <f t="shared" ref="J5:J28" si="1">_xlfn.CONCAT("66",B5,"000")</f>
+        <v>66005000</v>
+      </c>
+      <c r="K5" s="35"/>
+      <c r="L5" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="28"/>
+      <c r="P5" s="29"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" s="38"/>
+      <c r="F6" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>66006001</v>
+      </c>
+      <c r="J6" s="44" t="str">
+        <f t="shared" si="1"/>
+        <v>66006000</v>
+      </c>
+      <c r="K6" s="35"/>
+      <c r="L6" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" s="28"/>
+      <c r="P6" s="29"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="E7" s="38"/>
+      <c r="F7" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="I7" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>66012001</v>
+      </c>
+      <c r="J7" s="44" t="str">
+        <f t="shared" si="1"/>
+        <v>66012000</v>
+      </c>
+      <c r="K7" s="35"/>
+      <c r="L7" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="29"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>66011001</v>
+      </c>
+      <c r="J8" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v>66011000</v>
+      </c>
+      <c r="K8" s="36"/>
+      <c r="L8" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="M8" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="N8" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="O8" s="30"/>
+      <c r="P8" s="31"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="E9" s="37"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>66004001</v>
+      </c>
+      <c r="J9" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>66004000</v>
+      </c>
+      <c r="K9" s="34"/>
+      <c r="L9" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="M9" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="27"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="E10" s="38"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>66005001</v>
+      </c>
+      <c r="J10" s="44" t="str">
+        <f t="shared" si="1"/>
+        <v>66005000</v>
+      </c>
+      <c r="K10" s="35"/>
+      <c r="L10" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="M10" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="29"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>66006001</v>
+      </c>
+      <c r="J11" s="44" t="str">
+        <f t="shared" si="1"/>
+        <v>66006000</v>
+      </c>
+      <c r="K11" s="35"/>
+      <c r="L11" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="M11" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="29"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="E12" s="38"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>66012001</v>
+      </c>
+      <c r="J12" s="44" t="str">
+        <f t="shared" si="1"/>
+        <v>66012000</v>
+      </c>
+      <c r="K12" s="35"/>
+      <c r="L12" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="M12" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="29"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="E13" s="39"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>66011001</v>
+      </c>
+      <c r="J13" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v>66011000</v>
+      </c>
+      <c r="K13" s="36"/>
+      <c r="L13" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="M13" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="31"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" s="47"/>
+      <c r="F14" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="I14" s="49" t="str">
+        <f>_xlfn.CONCAT("66",B14,"001")</f>
+        <v>66004001</v>
+      </c>
+      <c r="J14" s="50" t="str">
+        <f>_xlfn.CONCAT("66",B14,"000")</f>
+        <v>66004000</v>
+      </c>
+      <c r="K14" s="51"/>
+      <c r="L14" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="M14" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="O14" s="48"/>
+      <c r="P14" s="52"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" s="54"/>
+      <c r="F15" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="56" t="str">
+        <f t="shared" ref="I15:I23" si="2">_xlfn.CONCAT("66",B15,"001")</f>
+        <v>66005001</v>
+      </c>
+      <c r="J15" s="57" t="str">
+        <f t="shared" ref="J15:J23" si="3">_xlfn.CONCAT("66",B15,"000")</f>
+        <v>66005000</v>
+      </c>
+      <c r="K15" s="58"/>
+      <c r="L15" s="55" t="s">
+        <v>212</v>
+      </c>
+      <c r="M15" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="N15" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="O15" s="55"/>
+      <c r="P15" s="59"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E16" s="54"/>
+      <c r="F16" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="56" t="str">
+        <f t="shared" si="2"/>
+        <v>66006001</v>
+      </c>
+      <c r="J16" s="57" t="str">
+        <f t="shared" si="3"/>
+        <v>66006000</v>
+      </c>
+      <c r="K16" s="58"/>
+      <c r="L16" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="M16" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="N16" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="O16" s="55"/>
+      <c r="P16" s="59"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E17" s="54"/>
+      <c r="F17" s="55" t="s">
+        <v>184</v>
+      </c>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55" t="s">
+        <v>184</v>
+      </c>
+      <c r="I17" s="56" t="str">
+        <f t="shared" si="2"/>
+        <v>66012001</v>
+      </c>
+      <c r="J17" s="57" t="str">
+        <f t="shared" si="3"/>
+        <v>66012000</v>
+      </c>
+      <c r="K17" s="58"/>
+      <c r="L17" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="M17" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" s="55"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="59"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="62" t="s">
+        <v>216</v>
+      </c>
+      <c r="E18" s="62"/>
+      <c r="F18" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="64" t="str">
+        <f t="shared" si="2"/>
+        <v>66011001</v>
+      </c>
+      <c r="J18" s="65" t="str">
+        <f t="shared" si="3"/>
+        <v>66011000</v>
+      </c>
+      <c r="K18" s="66"/>
+      <c r="L18" s="63" t="s">
+        <v>214</v>
+      </c>
+      <c r="M18" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="N18" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="O18" s="63"/>
+      <c r="P18" s="67"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="48"/>
+      <c r="D19" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="E19" s="47"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="49" t="str">
+        <f t="shared" si="2"/>
+        <v>66004001</v>
+      </c>
+      <c r="J19" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v>66004000</v>
+      </c>
+      <c r="K19" s="51"/>
+      <c r="L19" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="M19" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="N19" s="48"/>
+      <c r="O19" s="48"/>
+      <c r="P19" s="52"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="53" t="s">
+        <v>186</v>
+      </c>
+      <c r="B20" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="55"/>
+      <c r="D20" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E20" s="54"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="56" t="str">
+        <f t="shared" si="2"/>
+        <v>66005001</v>
+      </c>
+      <c r="J20" s="57" t="str">
+        <f t="shared" si="3"/>
+        <v>66005000</v>
+      </c>
+      <c r="K20" s="58"/>
+      <c r="L20" s="55" t="s">
+        <v>212</v>
+      </c>
+      <c r="M20" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="N20" s="55"/>
+      <c r="O20" s="55"/>
+      <c r="P20" s="59"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="55"/>
+      <c r="D21" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E21" s="54"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="56" t="str">
+        <f t="shared" si="2"/>
+        <v>66006001</v>
+      </c>
+      <c r="J21" s="57" t="str">
+        <f t="shared" si="3"/>
+        <v>66006000</v>
+      </c>
+      <c r="K21" s="58"/>
+      <c r="L21" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="M21" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="59"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="55"/>
+      <c r="D22" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E22" s="54"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="56" t="str">
+        <f t="shared" si="2"/>
+        <v>66012001</v>
+      </c>
+      <c r="J22" s="57" t="str">
+        <f t="shared" si="3"/>
+        <v>66012000</v>
+      </c>
+      <c r="K22" s="58"/>
+      <c r="L22" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="M22" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="59"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="63"/>
+      <c r="D23" s="62" t="s">
+        <v>216</v>
+      </c>
+      <c r="E23" s="62"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="64" t="str">
+        <f t="shared" si="2"/>
+        <v>66011001</v>
+      </c>
+      <c r="J23" s="65" t="str">
+        <f t="shared" si="3"/>
+        <v>66011000</v>
+      </c>
+      <c r="K23" s="66"/>
+      <c r="L23" s="63" t="s">
+        <v>214</v>
+      </c>
+      <c r="M23" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="N23" s="63"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="67"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="68" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="C24" s="69"/>
+      <c r="D24" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="49" t="str">
+        <f>_xlfn.CONCAT("66",B24,"0",D24)</f>
+        <v>66530101</v>
+      </c>
+      <c r="J24" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v>665301000</v>
+      </c>
+      <c r="K24" s="70"/>
+      <c r="L24" s="69" t="s">
+        <v>211</v>
+      </c>
+      <c r="M24" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="N24" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="O24" s="69" t="s">
+        <v>218</v>
+      </c>
+      <c r="P24" s="71" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="72" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>221</v>
+      </c>
+      <c r="C25" s="73"/>
+      <c r="D25" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E25" s="54" t="s">
+        <v>217</v>
+      </c>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="56" t="str">
+        <f t="shared" ref="I25:I28" si="4">_xlfn.CONCAT("66",B25,"0",D25)</f>
+        <v>66530201</v>
+      </c>
+      <c r="J25" s="57" t="str">
+        <f t="shared" si="1"/>
+        <v>665302000</v>
+      </c>
+      <c r="K25" s="74"/>
+      <c r="L25" s="73" t="s">
+        <v>212</v>
+      </c>
+      <c r="M25" s="73" t="s">
+        <v>47</v>
+      </c>
+      <c r="N25" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="O25" s="73" t="s">
+        <v>218</v>
+      </c>
+      <c r="P25" s="75" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="72" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>222</v>
+      </c>
+      <c r="C26" s="73"/>
+      <c r="D26" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E26" s="54" t="s">
+        <v>217</v>
+      </c>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="56" t="str">
+        <f t="shared" si="4"/>
+        <v>66530301</v>
+      </c>
+      <c r="J26" s="57" t="str">
+        <f t="shared" si="1"/>
+        <v>665303000</v>
+      </c>
+      <c r="K26" s="74"/>
+      <c r="L26" s="73" t="s">
+        <v>213</v>
+      </c>
+      <c r="M26" s="73" t="s">
+        <v>48</v>
+      </c>
+      <c r="N26" s="73" t="s">
+        <v>52</v>
+      </c>
+      <c r="O26" s="73" t="s">
+        <v>218</v>
+      </c>
+      <c r="P26" s="75" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="72" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" s="54" t="s">
+        <v>223</v>
+      </c>
+      <c r="C27" s="73"/>
+      <c r="D27" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27" s="54" t="s">
+        <v>217</v>
+      </c>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73"/>
+      <c r="I27" s="56" t="str">
+        <f t="shared" si="4"/>
+        <v>66535101</v>
+      </c>
+      <c r="J27" s="57" t="str">
+        <f t="shared" si="1"/>
+        <v>665351000</v>
+      </c>
+      <c r="K27" s="74"/>
+      <c r="L27" s="73" t="s">
+        <v>215</v>
+      </c>
+      <c r="M27" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="N27" s="73"/>
+      <c r="O27" s="73" t="s">
+        <v>218</v>
+      </c>
+      <c r="P27" s="75" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="B28" s="62" t="s">
+        <v>224</v>
+      </c>
+      <c r="C28" s="77"/>
+      <c r="D28" s="62" t="s">
+        <v>216</v>
+      </c>
+      <c r="E28" s="62" t="s">
+        <v>217</v>
+      </c>
+      <c r="F28" s="77"/>
+      <c r="G28" s="77"/>
+      <c r="H28" s="77"/>
+      <c r="I28" s="64" t="str">
+        <f t="shared" si="4"/>
+        <v>66535201</v>
+      </c>
+      <c r="J28" s="65" t="str">
+        <f t="shared" si="1"/>
+        <v>665352000</v>
+      </c>
+      <c r="K28" s="78"/>
+      <c r="L28" s="77" t="s">
+        <v>214</v>
+      </c>
+      <c r="M28" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="N28" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="O28" s="77" t="s">
+        <v>218</v>
+      </c>
+      <c r="P28" s="79" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="X31" sqref="X31"/>
     </sheetView>
@@ -1829,7 +3331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADDE2A7-CDFA-4D13-ACD7-212D5F91D52B}">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -2261,7 +3763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE9EA4D-4E90-422E-A935-2F982471E9B6}">
   <dimension ref="A1:D9"/>
   <sheetViews>

</xml_diff>